<commit_message>
proj1 and proj2 added
</commit_message>
<xml_diff>
--- a/PROJ1/marksheets/1401CB01.xlsx
+++ b/PROJ1/marksheets/1401CB01.xlsx
@@ -639,7 +639,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="8" t="n">
-        <v>-4</v>
+        <v>-1</v>
       </c>
       <c r="D11" s="5" t="n">
         <v>0</v>
@@ -656,12 +656,12 @@
         <v>56</v>
       </c>
       <c r="C12" s="8" t="n">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="D12" s="5" t="n"/>
       <c r="E12" s="9" t="inlineStr">
         <is>
-          <t>0/112</t>
+          <t>42/112</t>
         </is>
       </c>
     </row>

</xml_diff>